<commit_message>
ENDOXWEB - Corretta checklist test 32 e 40
Corretto file report-checklist.xlsx per test 32 e 40.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GRUPPOGPI00/TESI_SPA/ENDOXWEB/25.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111GRUPPOGPI00/TESI_SPA/ENDOXWEB/25.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bugs\FSE2_0\Accreditamento\ENDOX_ENDOXWEB_OPTINET\TESTCASE\ENDOXWEB\20240105\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348B6C9C-34B8-4CB9-8729-6E9E04161A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4EEBEC-7B6B-48CA-B7E1-767716E04725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2160" uniqueCount="891">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2162" uniqueCount="891">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -7708,10 +7708,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="D168" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="K169" sqref="K169"/>
+      <selection pane="bottomRight" activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7902,7 +7902,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="15"/>
     </row>
-    <row r="9" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>24</v>
       </c>
@@ -8950,7 +8950,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="141.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" ht="141.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="20">
         <v>32</v>
       </c>
@@ -8982,7 +8982,9 @@
         <v>138</v>
       </c>
       <c r="K39" s="25"/>
-      <c r="L39" s="25"/>
+      <c r="L39" s="25" t="s">
+        <v>847</v>
+      </c>
       <c r="M39" s="25" t="s">
         <v>138</v>
       </c>
@@ -9240,7 +9242,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="180" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="20">
         <v>40</v>
       </c>
@@ -9272,7 +9274,9 @@
         <v>138</v>
       </c>
       <c r="K47" s="25"/>
-      <c r="L47" s="25"/>
+      <c r="L47" s="25" t="s">
+        <v>847</v>
+      </c>
       <c r="M47" s="25" t="s">
         <v>138</v>
       </c>
@@ -9538,7 +9542,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="20">
         <v>48</v>
       </c>
@@ -13788,7 +13792,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="135" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="20">
         <v>169</v>
       </c>

</xml_diff>

<commit_message>
Accreditamento TESI SPA - ENDOXWEB - Rifatti test 32,40,160,161
Come da mail ricevuta oggi 18/01/2024 da FSE 2.0:
"Salve, Con la presente si comunica il mancato superamento dei seguenti test [160, 40, 161, 32] per il servizio [validazione/pubblicazione] del Fornitore [A1#111GRUPPOGPI00] - Vendor:[TESI_SPA] - ID: [ENDOXWEB] - Version: [25.0] - Sha: [2306db3c7af02a2127e33e3ebc6150a258c804d6] in data odierna.
Saluti,
Il Team FSE 2.0 "

sono stati rifatti test case 32,40,160,161
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GRUPPOGPI00/TESI_SPA/ENDOXWEB/25.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111GRUPPOGPI00/TESI_SPA/ENDOXWEB/25.0/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bugs\FSE2_0\Accreditamento\ENDOX_ENDOXWEB_OPTINET\TESTCASE\ENDOXWEB\20240105\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bugs\FSE2_0\Accreditamento\ENDOX_ENDOXWEB_OPTINET\TESTCASE\ENDOXWEB\20240118\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4EEBEC-7B6B-48CA-B7E1-767716E04725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B631E0EC-9138-4B89-9DCC-852316710BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -4700,15 +4700,6 @@
     <t>Il referto non è stato validato dal sistema, si desidera contnuare?</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.50504.4.4.18.56d1da87befe2b4e343b040253682ab96774e267e084581f6d511f6485171e6b.9d8d1320a0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-01-03T13:59:24.305Z</t>
-  </si>
-  <si>
-    <t>23afd723061e4346</t>
-  </si>
-  <si>
     <t>18203a19a407f970</t>
   </si>
   <si>
@@ -4724,19 +4715,7 @@
     <t xml:space="preserve"> il programma memorizza nel DB il messaggio di errore che proviene dal servizio di validazione per analisi successiva in backoffice. Una volta corretta la configurazione dell'integrazione (in questo caso il paramatero purpose_of_use)  l'utente dovrà rigenerare il referto e rifirmare</t>
   </si>
   <si>
-    <t>2024-01-05T08:38:07.100Z</t>
-  </si>
-  <si>
-    <t>28480377a3611f73</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
-  </si>
-  <si>
-    <t>d99f5c579c63a383</t>
-  </si>
-  <si>
-    <t>2024-01-05T08:54:15.576Z</t>
   </si>
   <si>
     <t>Il software non gestisce in modo strutturato l'informazione relativa alle procedure legate alle singole prestazioni. 
@@ -4781,6 +4760,27 @@
   </si>
   <si>
     <t>Questo test non è applicabile perché la sezione relativa al quesito diagnostico viene inserita nel CDA solo se è stata compilata la relatova sezione lato applicativo, quindi il text è sempre presente nel CDA nel caso sia stato compilato il quesito diagnostico.</t>
+  </si>
+  <si>
+    <t>2024-01-18T09:27:08.548Z</t>
+  </si>
+  <si>
+    <t>16f852b1fe511be3</t>
+  </si>
+  <si>
+    <t>728558af440259b3</t>
+  </si>
+  <si>
+    <t>2024-01-18T09:29:02.023Z</t>
+  </si>
+  <si>
+    <t>2024-01-18T09:32:16.918Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50504.4.4.18.56d1da87befe2b4e343b040253682ab96774e267e084581f6d511f6485171e6b.fb10d5bb1b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>3992be125ba30569</t>
   </si>
 </sst>
 </file>
@@ -7708,10 +7708,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E168" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="L39" sqref="L39"/>
+      <selection pane="bottomRight" activeCell="I168" sqref="I168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8967,16 +8967,16 @@
         <v>103</v>
       </c>
       <c r="F39" s="23">
-        <v>45296</v>
+        <v>45309</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>877</v>
+        <v>884</v>
       </c>
       <c r="H39" s="24" t="s">
-        <v>878</v>
+        <v>885</v>
       </c>
       <c r="I39" s="24" t="s">
-        <v>879</v>
+        <v>874</v>
       </c>
       <c r="J39" s="25" t="s">
         <v>138</v>
@@ -8995,7 +8995,7 @@
         <v>138</v>
       </c>
       <c r="P39" s="25" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="Q39" s="25"/>
       <c r="R39" s="26"/>
@@ -9259,16 +9259,16 @@
         <v>129</v>
       </c>
       <c r="F47" s="23">
-        <v>45296</v>
+        <v>45309</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>881</v>
+        <v>887</v>
       </c>
       <c r="H47" s="24" t="s">
-        <v>880</v>
+        <v>886</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>879</v>
+        <v>874</v>
       </c>
       <c r="J47" s="25" t="s">
         <v>138</v>
@@ -9287,7 +9287,7 @@
         <v>138</v>
       </c>
       <c r="P47" s="25" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="Q47" s="25"/>
       <c r="R47" s="26"/>
@@ -12948,7 +12948,7 @@
         <v>847</v>
       </c>
       <c r="K154" s="25" t="s">
-        <v>882</v>
+        <v>875</v>
       </c>
       <c r="L154" s="25"/>
       <c r="M154" s="25"/>
@@ -13100,7 +13100,7 @@
         <v>847</v>
       </c>
       <c r="K158" s="25" t="s">
-        <v>883</v>
+        <v>876</v>
       </c>
       <c r="L158" s="25"/>
       <c r="M158" s="25"/>
@@ -13380,7 +13380,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="20">
         <v>159</v>
       </c>
@@ -13418,7 +13418,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="405" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:20" ht="405.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="20">
         <v>160</v>
       </c>
@@ -13435,16 +13435,16 @@
         <v>363</v>
       </c>
       <c r="F167" s="23">
-        <v>45294</v>
+        <v>45309</v>
       </c>
       <c r="G167" s="24" t="s">
-        <v>870</v>
+        <v>888</v>
       </c>
       <c r="H167" s="24" t="s">
-        <v>871</v>
+        <v>890</v>
       </c>
       <c r="I167" s="24" t="s">
-        <v>869</v>
+        <v>889</v>
       </c>
       <c r="J167" s="25" t="s">
         <v>138</v>
@@ -13463,7 +13463,7 @@
         <v>138</v>
       </c>
       <c r="P167" s="25" t="s">
-        <v>884</v>
+        <v>877</v>
       </c>
       <c r="Q167" s="25"/>
       <c r="R167" s="26"/>
@@ -13472,7 +13472,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="405" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:20" ht="405.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="20">
         <v>161</v>
       </c>
@@ -13489,16 +13489,16 @@
         <v>365</v>
       </c>
       <c r="F168" s="23">
-        <v>45294</v>
+        <v>45309</v>
       </c>
       <c r="G168" s="24" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="H168" s="24" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="I168" s="24" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="J168" s="25" t="s">
         <v>138</v>
@@ -13517,7 +13517,7 @@
         <v>138</v>
       </c>
       <c r="P168" s="25" t="s">
-        <v>884</v>
+        <v>877</v>
       </c>
       <c r="Q168" s="25"/>
       <c r="R168" s="26"/>
@@ -13526,7 +13526,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="135" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="20">
         <v>162</v>
       </c>
@@ -13550,7 +13550,7 @@
         <v>847</v>
       </c>
       <c r="K169" s="25" t="s">
-        <v>890</v>
+        <v>883</v>
       </c>
       <c r="L169" s="25"/>
       <c r="M169" s="25"/>
@@ -13588,7 +13588,7 @@
         <v>847</v>
       </c>
       <c r="K170" s="25" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="L170" s="25"/>
       <c r="M170" s="25"/>
@@ -13626,7 +13626,7 @@
         <v>847</v>
       </c>
       <c r="K171" s="25" t="s">
-        <v>889</v>
+        <v>882</v>
       </c>
       <c r="L171" s="25"/>
       <c r="M171" s="25"/>
@@ -13664,7 +13664,7 @@
         <v>847</v>
       </c>
       <c r="K172" s="25" t="s">
-        <v>888</v>
+        <v>881</v>
       </c>
       <c r="L172" s="25"/>
       <c r="M172" s="25"/>
@@ -13702,7 +13702,7 @@
         <v>847</v>
       </c>
       <c r="K173" s="25" t="s">
-        <v>887</v>
+        <v>880</v>
       </c>
       <c r="L173" s="25"/>
       <c r="M173" s="25"/>
@@ -13740,7 +13740,7 @@
         <v>847</v>
       </c>
       <c r="K174" s="25" t="s">
-        <v>886</v>
+        <v>879</v>
       </c>
       <c r="L174" s="25"/>
       <c r="M174" s="25"/>
@@ -13778,7 +13778,7 @@
         <v>847</v>
       </c>
       <c r="K175" s="25" t="s">
-        <v>885</v>
+        <v>878</v>
       </c>
       <c r="L175" s="25"/>
       <c r="M175" s="25"/>

</xml_diff>

<commit_message>
Accreditamento TESI SPA - ENDOXWEB - Ripetuto test 161
Accreditamento TESI SPA - ENDOXWEB - Ripetuto test 161
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GRUPPOGPI00/TESI_SPA/ENDOXWEB/25.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111GRUPPOGPI00/TESI_SPA/ENDOXWEB/25.0/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bugs\FSE2_0\Accreditamento\ENDOX_ENDOXWEB_OPTINET\TESTCASE\ENDOXWEB\20240118\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bugs\FSE2_0\Accreditamento\ENDOX_ENDOXWEB_OPTINET\TESTCASE\ENDOXWEB\20240122\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B631E0EC-9138-4B89-9DCC-852316710BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC926C47-4783-48DE-8515-BB4D048387E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4700,15 +4700,6 @@
     <t>Il referto non è stato validato dal sistema, si desidera contnuare?</t>
   </si>
   <si>
-    <t>18203a19a407f970</t>
-  </si>
-  <si>
-    <t>2024-01-03T14:26:34.437Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.50504.4.4.18.8b5783d7291cb3213d104c0fb9af24903614858af615ec435c06fb02e9277195.556ac4ad6f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Questo test non è applicabile perché lato applicativo non è gestito l'inserimento delle procedure legate alla singola prestazione.</t>
   </si>
   <si>
@@ -4781,6 +4772,15 @@
   </si>
   <si>
     <t>3992be125ba30569</t>
+  </si>
+  <si>
+    <t>ffd256d40333bd1c</t>
+  </si>
+  <si>
+    <t>2024-01-22T09:32:55.961Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50504.4.4.18.8b5783d7291cb3213d104c0fb9af24903614858af615ec435c06fb02e9277195.9d5e099ceb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -7708,10 +7708,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E168" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E167" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I168" sqref="I168"/>
+      <selection pane="bottomRight" activeCell="G167" sqref="G167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8970,13 +8970,13 @@
         <v>45309</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
       <c r="H39" s="24" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
       <c r="I39" s="24" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="J39" s="25" t="s">
         <v>138</v>
@@ -8995,7 +8995,7 @@
         <v>138</v>
       </c>
       <c r="P39" s="25" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="Q39" s="25"/>
       <c r="R39" s="26"/>
@@ -9262,13 +9262,13 @@
         <v>45309</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
       <c r="H47" s="24" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="J47" s="25" t="s">
         <v>138</v>
@@ -9287,7 +9287,7 @@
         <v>138</v>
       </c>
       <c r="P47" s="25" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="Q47" s="25"/>
       <c r="R47" s="26"/>
@@ -12948,7 +12948,7 @@
         <v>847</v>
       </c>
       <c r="K154" s="25" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="L154" s="25"/>
       <c r="M154" s="25"/>
@@ -13100,7 +13100,7 @@
         <v>847</v>
       </c>
       <c r="K158" s="25" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="L158" s="25"/>
       <c r="M158" s="25"/>
@@ -13438,13 +13438,13 @@
         <v>45309</v>
       </c>
       <c r="G167" s="24" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="H167" s="24" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
       <c r="I167" s="24" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="J167" s="25" t="s">
         <v>138</v>
@@ -13463,7 +13463,7 @@
         <v>138</v>
       </c>
       <c r="P167" s="25" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="Q167" s="25"/>
       <c r="R167" s="26"/>
@@ -13489,16 +13489,16 @@
         <v>365</v>
       </c>
       <c r="F168" s="23">
-        <v>45309</v>
+        <v>45313</v>
       </c>
       <c r="G168" s="24" t="s">
-        <v>870</v>
+        <v>889</v>
       </c>
       <c r="H168" s="24" t="s">
-        <v>869</v>
+        <v>888</v>
       </c>
       <c r="I168" s="24" t="s">
-        <v>871</v>
+        <v>890</v>
       </c>
       <c r="J168" s="25" t="s">
         <v>138</v>
@@ -13517,7 +13517,7 @@
         <v>138</v>
       </c>
       <c r="P168" s="25" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="Q168" s="25"/>
       <c r="R168" s="26"/>
@@ -13550,7 +13550,7 @@
         <v>847</v>
       </c>
       <c r="K169" s="25" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
       <c r="L169" s="25"/>
       <c r="M169" s="25"/>
@@ -13588,7 +13588,7 @@
         <v>847</v>
       </c>
       <c r="K170" s="25" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="L170" s="25"/>
       <c r="M170" s="25"/>
@@ -13626,7 +13626,7 @@
         <v>847</v>
       </c>
       <c r="K171" s="25" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="L171" s="25"/>
       <c r="M171" s="25"/>
@@ -13664,7 +13664,7 @@
         <v>847</v>
       </c>
       <c r="K172" s="25" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
       <c r="L172" s="25"/>
       <c r="M172" s="25"/>
@@ -13702,7 +13702,7 @@
         <v>847</v>
       </c>
       <c r="K173" s="25" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="L173" s="25"/>
       <c r="M173" s="25"/>
@@ -13740,7 +13740,7 @@
         <v>847</v>
       </c>
       <c r="K174" s="25" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
       <c r="L174" s="25"/>
       <c r="M174" s="25"/>
@@ -13778,7 +13778,7 @@
         <v>847</v>
       </c>
       <c r="K175" s="25" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="L175" s="25"/>
       <c r="M175" s="25"/>

</xml_diff>

<commit_message>
A1#111GRUPPOGPI00-TESI_SPA-ENDOXWEB-25.0 - Ripetuti Test 32-40-160-161
In riferimento alla issue #573, sono stati ripetuti i test case 32-40-160-161 in quanto le precedenti chiamate di validazione verso Gateway erano state fatte con applicationID errato ("OPTINET" invece che "ENDOXWEB")
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GRUPPOGPI00/TESI_SPA/ENDOXWEB/25.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111GRUPPOGPI00/TESI_SPA/ENDOXWEB/25.0/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bugs\FSE2_0\Accreditamento\ENDOX_ENDOXWEB_OPTINET\TESTCASE\ENDOXWEB\20240122\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bugs\FSE2_0\Accreditamento\ENDOX_ENDOXWEB_OPTINET\TESTCASE\ENDOXWEB\20240131\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC926C47-4783-48DE-8515-BB4D048387E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1F2429-C159-4E6C-B515-027F531799B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -4753,34 +4753,34 @@
     <t>Questo test non è applicabile perché la sezione relativa al quesito diagnostico viene inserita nel CDA solo se è stata compilata la relatova sezione lato applicativo, quindi il text è sempre presente nel CDA nel caso sia stato compilato il quesito diagnostico.</t>
   </si>
   <si>
-    <t>2024-01-18T09:27:08.548Z</t>
-  </si>
-  <si>
-    <t>16f852b1fe511be3</t>
-  </si>
-  <si>
-    <t>728558af440259b3</t>
-  </si>
-  <si>
-    <t>2024-01-18T09:29:02.023Z</t>
-  </si>
-  <si>
-    <t>2024-01-18T09:32:16.918Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.50504.4.4.18.56d1da87befe2b4e343b040253682ab96774e267e084581f6d511f6485171e6b.fb10d5bb1b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>3992be125ba30569</t>
-  </si>
-  <si>
-    <t>ffd256d40333bd1c</t>
-  </si>
-  <si>
-    <t>2024-01-22T09:32:55.961Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.50504.4.4.18.8b5783d7291cb3213d104c0fb9af24903614858af615ec435c06fb02e9277195.9d5e099ceb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>c178b7a831a83db6</t>
+  </si>
+  <si>
+    <t>2024-01-31T08:15:15.349Z</t>
+  </si>
+  <si>
+    <t>3b8a839017abfb5f</t>
+  </si>
+  <si>
+    <t>2024-01-31T08:17:27.592Z</t>
+  </si>
+  <si>
+    <t>e2a49463fb3a0920</t>
+  </si>
+  <si>
+    <t>2024-01-31T08:19:34.905Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50504.4.4.18.56d1da87befe2b4e343b040253682ab96774e267e084581f6d511f6485171e6b.655c247abb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>4c6b97a9351f6825</t>
+  </si>
+  <si>
+    <t>2024-01-31T08:21:32.798Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50504.4.4.18.8b5783d7291cb3213d104c0fb9af24903614858af615ec435c06fb02e9277195.060f1dec63^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -7708,10 +7708,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E167" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E168" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="G167" sqref="G167"/>
+      <selection pane="bottomRight" activeCell="I168" sqref="I168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8967,13 +8967,13 @@
         <v>103</v>
       </c>
       <c r="F39" s="23">
-        <v>45309</v>
+        <v>45322</v>
       </c>
       <c r="G39" s="24" t="s">
+        <v>882</v>
+      </c>
+      <c r="H39" s="24" t="s">
         <v>881</v>
-      </c>
-      <c r="H39" s="24" t="s">
-        <v>882</v>
       </c>
       <c r="I39" s="24" t="s">
         <v>871</v>
@@ -9259,7 +9259,7 @@
         <v>129</v>
       </c>
       <c r="F47" s="23">
-        <v>45309</v>
+        <v>45322</v>
       </c>
       <c r="G47" s="24" t="s">
         <v>884</v>
@@ -13435,16 +13435,16 @@
         <v>363</v>
       </c>
       <c r="F167" s="23">
-        <v>45309</v>
+        <v>45322</v>
       </c>
       <c r="G167" s="24" t="s">
+        <v>886</v>
+      </c>
+      <c r="H167" s="24" t="s">
         <v>885</v>
       </c>
-      <c r="H167" s="24" t="s">
+      <c r="I167" s="24" t="s">
         <v>887</v>
-      </c>
-      <c r="I167" s="24" t="s">
-        <v>886</v>
       </c>
       <c r="J167" s="25" t="s">
         <v>138</v>
@@ -13489,7 +13489,7 @@
         <v>365</v>
       </c>
       <c r="F168" s="23">
-        <v>45313</v>
+        <v>45322</v>
       </c>
       <c r="G168" s="24" t="s">
         <v>889</v>

</xml_diff>